<commit_message>
minor changes along side
</commit_message>
<xml_diff>
--- a/data/Guildes_revues_ER.xlsx
+++ b/data/Guildes_revues_ER.xlsx
@@ -7192,10 +7192,10 @@
   <dimension ref="A1:AD31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L27" sqref="L27"/>
+      <selection pane="bottomRight" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7594,10 +7594,10 @@
         <v>1876</v>
       </c>
       <c r="O5" s="125" t="s">
+        <v>1876</v>
+      </c>
+      <c r="P5" s="125" t="s">
         <v>1879</v>
-      </c>
-      <c r="P5" s="125" t="s">
-        <v>1876</v>
       </c>
       <c r="Q5" s="125" t="s">
         <v>1876</v>

</xml_diff>

<commit_message>
integrate factsheet into master modelling
</commit_message>
<xml_diff>
--- a/data/Guildes_revues_ER.xlsx
+++ b/data/Guildes_revues_ER.xlsx
@@ -7192,10 +7192,10 @@
   <dimension ref="A1:AD31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="H14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O5" sqref="O5"/>
+      <selection pane="bottomRight" activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7594,7 +7594,7 @@
         <v>1876</v>
       </c>
       <c r="O5" s="125" t="s">
-        <v>1876</v>
+        <v>1879</v>
       </c>
       <c r="P5" s="125" t="s">
         <v>1879</v>
@@ -8227,7 +8227,7 @@
         <v>1879</v>
       </c>
       <c r="P14" s="125" t="s">
-        <v>1876</v>
+        <v>1879</v>
       </c>
       <c r="Q14" s="125" t="s">
         <v>1876</v>
@@ -8509,7 +8509,7 @@
         <v>1879</v>
       </c>
       <c r="P18" s="125" t="s">
-        <v>1876</v>
+        <v>1879</v>
       </c>
       <c r="Q18" s="125" t="s">
         <v>1876</v>
@@ -8626,10 +8626,10 @@
         <v>1876</v>
       </c>
       <c r="O20" s="125" t="s">
+        <v>1879</v>
+      </c>
+      <c r="P20" s="125" t="s">
         <v>1876</v>
-      </c>
-      <c r="P20" s="125" t="s">
-        <v>1879</v>
       </c>
       <c r="Q20" s="125" t="s">
         <v>1876</v>
@@ -8638,7 +8638,7 @@
         <v>1878</v>
       </c>
       <c r="S20" s="125">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="T20" s="1">
         <v>750</v>
@@ -8705,7 +8705,7 @@
         <v>1876</v>
       </c>
       <c r="O21" s="125" t="s">
-        <v>1876</v>
+        <v>1879</v>
       </c>
       <c r="P21" s="125" t="s">
         <v>1879</v>
@@ -8837,7 +8837,7 @@
         <v>1876</v>
       </c>
       <c r="O23" s="125" t="s">
-        <v>1876</v>
+        <v>1879</v>
       </c>
       <c r="P23" s="125" t="s">
         <v>1879</v>

</xml_diff>

<commit_message>
Add priorisation part and updated IFN bioindex
</commit_message>
<xml_diff>
--- a/data/Guildes_revues_ER.xlsx
+++ b/data/Guildes_revues_ER.xlsx
@@ -7074,10 +7074,10 @@
   <dimension ref="A1:AD31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P26" sqref="P26"/>
+      <selection pane="bottomRight" activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -7859,7 +7859,7 @@
         <v>1850</v>
       </c>
       <c r="P11" s="113" t="s">
-        <v>1847</v>
+        <v>1850</v>
       </c>
       <c r="Q11" s="113" t="s">
         <v>1847</v>

</xml_diff>